<commit_message>
organization and updated data dictionary
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -566,7 +566,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -583,6 +583,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b val="1"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color indexed="14"/>
       <name val="Calibri (Body)"/>
@@ -594,6 +600,7 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b val="1"/>
       <sz val="12"/>
       <color indexed="18"/>
       <name val="Calibri"/>
@@ -789,7 +796,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -811,37 +818,46 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -856,19 +872,22 @@
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -883,10 +902,10 @@
     <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -901,7 +920,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2168,7 +2187,7 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" ht="15.35" customHeight="1">
-      <c r="A7" t="s" s="7">
+      <c r="A7" t="s" s="11">
         <v>23</v>
       </c>
       <c r="B7" t="s" s="8">
@@ -2272,24 +2291,24 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
-      <c r="A11" t="s" s="11">
+      <c r="A11" t="s" s="12">
         <v>31</v>
       </c>
-      <c r="B11" t="s" s="12">
+      <c r="B11" t="s" s="13">
         <v>32</v>
       </c>
-      <c r="C11" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s" s="12">
+      <c r="C11" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" t="s" s="12">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" t="s" s="13">
         <v>34</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="10"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -2298,24 +2317,24 @@
       <c r="N11" s="3"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
-      <c r="A12" t="s" s="11">
+      <c r="A12" t="s" s="12">
         <v>35</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="B12" t="s" s="13">
         <v>36</v>
       </c>
-      <c r="C12" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s" s="12">
+      <c r="C12" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" t="s" s="12">
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" t="s" s="13">
         <v>34</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="10"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -2324,24 +2343,24 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
-      <c r="A13" t="s" s="11">
+      <c r="A13" t="s" s="12">
         <v>37</v>
       </c>
-      <c r="B13" t="s" s="12">
+      <c r="B13" t="s" s="13">
         <v>38</v>
       </c>
-      <c r="C13" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s" s="12">
+      <c r="C13" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" t="s" s="12">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" t="s" s="13">
         <v>34</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="10"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -2350,26 +2369,26 @@
       <c r="N13" s="3"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
-      <c r="A14" t="s" s="11">
+      <c r="A14" t="s" s="12">
         <v>39</v>
       </c>
-      <c r="B14" t="s" s="12">
+      <c r="B14" t="s" s="13">
         <v>40</v>
       </c>
-      <c r="C14" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s" s="12">
+      <c r="C14" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E14" t="s" s="12">
+      <c r="E14" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" t="s" s="12">
+      <c r="F14" s="14"/>
+      <c r="G14" t="s" s="13">
         <v>34</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="10"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -2404,7 +2423,7 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
-      <c r="A16" t="s" s="7">
+      <c r="A16" t="s" s="11">
         <v>45</v>
       </c>
       <c r="B16" t="s" s="8">
@@ -2430,24 +2449,24 @@
       <c r="N16" s="3"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
-      <c r="A17" t="s" s="14">
+      <c r="A17" t="s" s="15">
         <v>47</v>
       </c>
-      <c r="B17" t="s" s="15">
+      <c r="B17" t="s" s="16">
         <v>48</v>
       </c>
-      <c r="C17" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s" s="15">
+      <c r="C17" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" t="s" s="15">
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="H17" s="16"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="10"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -2456,24 +2475,24 @@
       <c r="N17" s="3"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
-      <c r="A18" t="s" s="14">
+      <c r="A18" t="s" s="15">
         <v>51</v>
       </c>
-      <c r="B18" t="s" s="15">
+      <c r="B18" t="s" s="16">
         <v>52</v>
       </c>
-      <c r="C18" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s" s="15">
+      <c r="C18" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" t="s" s="15">
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="H18" s="16"/>
+      <c r="H18" s="17"/>
       <c r="I18" s="10"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -2482,26 +2501,26 @@
       <c r="N18" s="3"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
-      <c r="A19" t="s" s="14">
+      <c r="A19" t="s" s="15">
         <v>53</v>
       </c>
-      <c r="B19" t="s" s="15">
+      <c r="B19" t="s" s="16">
         <v>54</v>
       </c>
-      <c r="C19" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s" s="15">
+      <c r="C19" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E19" t="s" s="15">
+      <c r="E19" t="s" s="16">
         <v>55</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" t="s" s="15">
+      <c r="F19" s="17"/>
+      <c r="G19" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="H19" s="16"/>
+      <c r="H19" s="17"/>
       <c r="I19" s="10"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2510,26 +2529,26 @@
       <c r="N19" s="3"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
-      <c r="A20" t="s" s="14">
+      <c r="A20" t="s" s="15">
         <v>56</v>
       </c>
-      <c r="B20" t="s" s="15">
+      <c r="B20" t="s" s="16">
         <v>57</v>
       </c>
-      <c r="C20" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s" s="15">
+      <c r="C20" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E20" t="s" s="15">
+      <c r="E20" t="s" s="16">
         <v>58</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" t="s" s="15">
+      <c r="F20" s="17"/>
+      <c r="G20" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="H20" s="16"/>
+      <c r="H20" s="17"/>
       <c r="I20" s="10"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2538,26 +2557,26 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
-      <c r="A21" t="s" s="14">
+      <c r="A21" t="s" s="18">
         <v>59</v>
       </c>
-      <c r="B21" t="s" s="15">
+      <c r="B21" t="s" s="16">
         <v>60</v>
       </c>
-      <c r="C21" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s" s="15">
+      <c r="C21" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E21" t="s" s="15">
+      <c r="E21" t="s" s="16">
         <v>60</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" t="s" s="15">
+      <c r="F21" s="17"/>
+      <c r="G21" t="s" s="16">
         <v>61</v>
       </c>
-      <c r="H21" s="16"/>
+      <c r="H21" s="17"/>
       <c r="I21" s="10"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2566,26 +2585,26 @@
       <c r="N21" s="3"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
-      <c r="A22" t="s" s="14">
+      <c r="A22" t="s" s="15">
         <v>62</v>
       </c>
-      <c r="B22" t="s" s="15">
+      <c r="B22" t="s" s="16">
         <v>63</v>
       </c>
-      <c r="C22" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s" s="15">
+      <c r="C22" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E22" t="s" s="15">
+      <c r="E22" t="s" s="16">
         <v>63</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" t="s" s="15">
+      <c r="F22" s="17"/>
+      <c r="G22" t="s" s="16">
         <v>61</v>
       </c>
-      <c r="H22" s="16"/>
+      <c r="H22" s="17"/>
       <c r="I22" s="10"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -2594,26 +2613,26 @@
       <c r="N22" s="3"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
-      <c r="A23" t="s" s="14">
+      <c r="A23" t="s" s="15">
         <v>64</v>
       </c>
-      <c r="B23" t="s" s="15">
+      <c r="B23" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="C23" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s" s="15">
+      <c r="C23" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E23" t="s" s="15">
+      <c r="E23" t="s" s="16">
         <v>65</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" t="s" s="15">
+      <c r="F23" s="17"/>
+      <c r="G23" t="s" s="16">
         <v>61</v>
       </c>
-      <c r="H23" s="16"/>
+      <c r="H23" s="17"/>
       <c r="I23" s="10"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -2622,26 +2641,26 @@
       <c r="N23" s="3"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
-      <c r="A24" t="s" s="14">
+      <c r="A24" t="s" s="15">
         <v>66</v>
       </c>
-      <c r="B24" t="s" s="15">
+      <c r="B24" t="s" s="16">
         <v>67</v>
       </c>
-      <c r="C24" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s" s="15">
+      <c r="C24" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E24" t="s" s="15">
+      <c r="E24" t="s" s="16">
         <v>67</v>
       </c>
-      <c r="F24" s="16"/>
-      <c r="G24" t="s" s="15">
+      <c r="F24" s="17"/>
+      <c r="G24" t="s" s="16">
         <v>61</v>
       </c>
-      <c r="H24" s="16"/>
+      <c r="H24" s="17"/>
       <c r="I24" s="10"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2650,26 +2669,26 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
-      <c r="A25" t="s" s="11">
+      <c r="A25" t="s" s="12">
         <v>68</v>
       </c>
-      <c r="B25" t="s" s="12">
+      <c r="B25" t="s" s="13">
         <v>69</v>
       </c>
-      <c r="C25" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s" s="12">
+      <c r="C25" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E25" t="s" s="12">
+      <c r="E25" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" t="s" s="12">
+      <c r="F25" s="14"/>
+      <c r="G25" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H25" s="13"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="10"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2678,26 +2697,26 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
-      <c r="A26" t="s" s="14">
+      <c r="A26" t="s" s="18">
         <v>70</v>
       </c>
-      <c r="B26" t="s" s="15">
+      <c r="B26" t="s" s="16">
         <v>71</v>
       </c>
-      <c r="C26" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D26" t="s" s="15">
+      <c r="C26" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E26" t="s" s="15">
+      <c r="E26" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="F26" s="16"/>
-      <c r="G26" t="s" s="15">
+      <c r="F26" s="17"/>
+      <c r="G26" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="H26" s="16"/>
+      <c r="H26" s="17"/>
       <c r="I26" s="10"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -2706,26 +2725,26 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
-      <c r="A27" t="s" s="14">
+      <c r="A27" t="s" s="18">
         <v>72</v>
       </c>
-      <c r="B27" t="s" s="15">
+      <c r="B27" t="s" s="16">
         <v>73</v>
       </c>
-      <c r="C27" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="D27" t="s" s="15">
+      <c r="C27" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s" s="16">
         <v>49</v>
       </c>
-      <c r="E27" t="s" s="15">
+      <c r="E27" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" t="s" s="15">
+      <c r="F27" s="17"/>
+      <c r="G27" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="H27" s="16"/>
+      <c r="H27" s="17"/>
       <c r="I27" s="10"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -2734,26 +2753,26 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
-      <c r="A28" t="s" s="11">
+      <c r="A28" t="s" s="19">
         <v>74</v>
       </c>
-      <c r="B28" t="s" s="12">
+      <c r="B28" t="s" s="13">
         <v>75</v>
       </c>
-      <c r="C28" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D28" t="s" s="12">
+      <c r="C28" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E28" t="s" s="12">
+      <c r="E28" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" t="s" s="12">
+      <c r="F28" s="14"/>
+      <c r="G28" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="10"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
@@ -2762,26 +2781,26 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
-      <c r="A29" t="s" s="11">
+      <c r="A29" t="s" s="12">
         <v>76</v>
       </c>
-      <c r="B29" t="s" s="12">
+      <c r="B29" t="s" s="13">
         <v>77</v>
       </c>
-      <c r="C29" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s" s="12">
+      <c r="C29" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E29" t="s" s="12">
+      <c r="E29" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" t="s" s="12">
+      <c r="F29" s="14"/>
+      <c r="G29" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="14"/>
       <c r="I29" s="10"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -2790,26 +2809,26 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
-      <c r="A30" t="s" s="11">
+      <c r="A30" t="s" s="12">
         <v>78</v>
       </c>
-      <c r="B30" t="s" s="12">
+      <c r="B30" t="s" s="13">
         <v>79</v>
       </c>
-      <c r="C30" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s" s="12">
+      <c r="C30" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E30" t="s" s="12">
+      <c r="E30" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" t="s" s="12">
+      <c r="F30" s="14"/>
+      <c r="G30" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H30" s="13"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="10"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2818,26 +2837,26 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
-      <c r="A31" t="s" s="11">
+      <c r="A31" t="s" s="19">
         <v>80</v>
       </c>
-      <c r="B31" t="s" s="12">
+      <c r="B31" t="s" s="13">
         <v>81</v>
       </c>
-      <c r="C31" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D31" t="s" s="12">
+      <c r="C31" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E31" t="s" s="12">
+      <c r="E31" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" t="s" s="12">
+      <c r="F31" s="14"/>
+      <c r="G31" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H31" s="13"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="10"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -2846,26 +2865,26 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
-      <c r="A32" t="s" s="11">
+      <c r="A32" t="s" s="19">
         <v>82</v>
       </c>
-      <c r="B32" t="s" s="12">
+      <c r="B32" t="s" s="13">
         <v>83</v>
       </c>
-      <c r="C32" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D32" t="s" s="12">
+      <c r="C32" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E32" t="s" s="12">
+      <c r="E32" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" t="s" s="12">
+      <c r="F32" s="14"/>
+      <c r="G32" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="10"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -2874,26 +2893,26 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
-      <c r="A33" t="s" s="11">
+      <c r="A33" t="s" s="19">
         <v>84</v>
       </c>
-      <c r="B33" t="s" s="12">
+      <c r="B33" t="s" s="13">
         <v>85</v>
       </c>
-      <c r="C33" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D33" t="s" s="12">
+      <c r="C33" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E33" t="s" s="12">
+      <c r="E33" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" t="s" s="12">
+      <c r="F33" s="14"/>
+      <c r="G33" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="14"/>
       <c r="I33" s="10"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -2902,26 +2921,26 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
-      <c r="A34" t="s" s="11">
+      <c r="A34" t="s" s="19">
         <v>86</v>
       </c>
-      <c r="B34" t="s" s="12">
+      <c r="B34" t="s" s="13">
         <v>87</v>
       </c>
-      <c r="C34" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D34" t="s" s="12">
+      <c r="C34" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E34" t="s" s="12">
+      <c r="E34" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" t="s" s="12">
+      <c r="F34" s="14"/>
+      <c r="G34" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H34" s="13"/>
+      <c r="H34" s="14"/>
       <c r="I34" s="10"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -2930,26 +2949,26 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
-      <c r="A35" t="s" s="11">
+      <c r="A35" t="s" s="19">
         <v>88</v>
       </c>
-      <c r="B35" t="s" s="12">
+      <c r="B35" t="s" s="13">
         <v>89</v>
       </c>
-      <c r="C35" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D35" t="s" s="12">
+      <c r="C35" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E35" t="s" s="12">
+      <c r="E35" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F35" s="13"/>
-      <c r="G35" t="s" s="12">
+      <c r="F35" s="14"/>
+      <c r="G35" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H35" s="13"/>
+      <c r="H35" s="14"/>
       <c r="I35" s="10"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
@@ -2958,26 +2977,26 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
-      <c r="A36" t="s" s="11">
+      <c r="A36" t="s" s="19">
         <v>90</v>
       </c>
-      <c r="B36" t="s" s="12">
+      <c r="B36" t="s" s="13">
         <v>91</v>
       </c>
-      <c r="C36" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s" s="12">
+      <c r="C36" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E36" t="s" s="12">
+      <c r="E36" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F36" s="13"/>
-      <c r="G36" t="s" s="12">
+      <c r="F36" s="14"/>
+      <c r="G36" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H36" s="13"/>
+      <c r="H36" s="14"/>
       <c r="I36" s="10"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -2986,28 +3005,28 @@
       <c r="N36" s="3"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
-      <c r="A37" t="s" s="11">
+      <c r="A37" t="s" s="12">
         <v>92</v>
       </c>
-      <c r="B37" t="s" s="12">
+      <c r="B37" t="s" s="13">
         <v>93</v>
       </c>
-      <c r="C37" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D37" t="s" s="12">
+      <c r="C37" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E37" t="s" s="12">
+      <c r="E37" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F37" t="s" s="12">
+      <c r="F37" t="s" s="13">
         <v>94</v>
       </c>
-      <c r="G37" t="s" s="12">
+      <c r="G37" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H37" s="13"/>
+      <c r="H37" s="14"/>
       <c r="I37" s="10"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -3016,28 +3035,28 @@
       <c r="N37" s="3"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
-      <c r="A38" t="s" s="11">
+      <c r="A38" t="s" s="12">
         <v>95</v>
       </c>
-      <c r="B38" t="s" s="12">
+      <c r="B38" t="s" s="13">
         <v>96</v>
       </c>
-      <c r="C38" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D38" t="s" s="12">
+      <c r="C38" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E38" t="s" s="12">
+      <c r="E38" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F38" t="s" s="12">
+      <c r="F38" t="s" s="13">
         <v>94</v>
       </c>
-      <c r="G38" t="s" s="12">
+      <c r="G38" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H38" s="13"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="10"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -3046,28 +3065,28 @@
       <c r="N38" s="3"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
-      <c r="A39" t="s" s="11">
+      <c r="A39" t="s" s="12">
         <v>97</v>
       </c>
-      <c r="B39" t="s" s="12">
+      <c r="B39" t="s" s="13">
         <v>98</v>
       </c>
-      <c r="C39" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s" s="12">
+      <c r="C39" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E39" t="s" s="12">
+      <c r="E39" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="F39" t="s" s="12">
+      <c r="F39" t="s" s="13">
         <v>94</v>
       </c>
-      <c r="G39" t="s" s="12">
+      <c r="G39" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="H39" s="13"/>
+      <c r="H39" s="14"/>
       <c r="I39" s="10"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -3076,24 +3095,24 @@
       <c r="N39" s="3"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
-      <c r="A40" t="s" s="11">
+      <c r="A40" t="s" s="12">
         <v>99</v>
       </c>
-      <c r="B40" t="s" s="12">
+      <c r="B40" t="s" s="13">
         <v>100</v>
       </c>
-      <c r="C40" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D40" t="s" s="12">
+      <c r="C40" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E40" t="s" s="12">
+      <c r="E40" t="s" s="13">
         <v>101</v>
       </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="10"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -3102,24 +3121,24 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
-      <c r="A41" t="s" s="11">
+      <c r="A41" t="s" s="12">
         <v>102</v>
       </c>
-      <c r="B41" t="s" s="12">
+      <c r="B41" t="s" s="13">
         <v>103</v>
       </c>
-      <c r="C41" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s" s="12">
+      <c r="C41" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E41" t="s" s="12">
+      <c r="E41" t="s" s="13">
         <v>104</v>
       </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
       <c r="I41" s="10"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
@@ -3128,24 +3147,24 @@
       <c r="N41" s="3"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
-      <c r="A42" t="s" s="11">
+      <c r="A42" t="s" s="12">
         <v>105</v>
       </c>
-      <c r="B42" t="s" s="12">
+      <c r="B42" t="s" s="13">
         <v>106</v>
       </c>
-      <c r="C42" t="s" s="12">
-        <v>9</v>
-      </c>
-      <c r="D42" t="s" s="12">
+      <c r="C42" t="s" s="13">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="E42" t="s" s="12">
+      <c r="E42" t="s" s="13">
         <v>107</v>
       </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
       <c r="I42" s="10"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -3168,7 +3187,7 @@
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
-      <c r="G43" t="s" s="17">
+      <c r="G43" t="s" s="20">
         <v>110</v>
       </c>
       <c r="H43" s="9"/>
@@ -3180,24 +3199,24 @@
       <c r="N43" s="3"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
-      <c r="A44" t="s" s="18">
+      <c r="A44" t="s" s="21">
         <v>111</v>
       </c>
-      <c r="B44" t="s" s="19">
+      <c r="B44" t="s" s="22">
         <v>112</v>
       </c>
-      <c r="C44" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s" s="19">
+      <c r="C44" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" t="s" s="19">
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H44" s="20"/>
+      <c r="H44" s="23"/>
       <c r="I44" s="10"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
@@ -3206,24 +3225,24 @@
       <c r="N44" s="3"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
-      <c r="A45" t="s" s="18">
+      <c r="A45" t="s" s="21">
         <v>115</v>
       </c>
-      <c r="B45" t="s" s="19">
+      <c r="B45" t="s" s="22">
         <v>116</v>
       </c>
-      <c r="C45" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D45" t="s" s="19">
+      <c r="C45" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" t="s" s="19">
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H45" s="20"/>
+      <c r="H45" s="23"/>
       <c r="I45" s="10"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -3232,24 +3251,24 @@
       <c r="N45" s="3"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
-      <c r="A46" t="s" s="18">
+      <c r="A46" t="s" s="21">
         <v>117</v>
       </c>
-      <c r="B46" t="s" s="19">
+      <c r="B46" t="s" s="22">
         <v>118</v>
       </c>
-      <c r="C46" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s" s="19">
+      <c r="C46" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" t="s" s="19">
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H46" s="20"/>
+      <c r="H46" s="23"/>
       <c r="I46" s="10"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -3258,24 +3277,24 @@
       <c r="N46" s="3"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
-      <c r="A47" t="s" s="18">
+      <c r="A47" t="s" s="21">
         <v>119</v>
       </c>
-      <c r="B47" t="s" s="19">
+      <c r="B47" t="s" s="22">
         <v>120</v>
       </c>
-      <c r="C47" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s" s="19">
+      <c r="C47" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" t="s" s="19">
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="G47" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H47" s="20"/>
+      <c r="H47" s="23"/>
       <c r="I47" s="10"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -3284,24 +3303,24 @@
       <c r="N47" s="3"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
-      <c r="A48" t="s" s="18">
+      <c r="A48" t="s" s="21">
         <v>121</v>
       </c>
-      <c r="B48" t="s" s="19">
+      <c r="B48" t="s" s="22">
         <v>122</v>
       </c>
-      <c r="C48" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s" s="19">
+      <c r="C48" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" t="s" s="19">
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H48" s="20"/>
+      <c r="H48" s="23"/>
       <c r="I48" s="10"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -3310,24 +3329,24 @@
       <c r="N48" s="3"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
-      <c r="A49" t="s" s="18">
+      <c r="A49" t="s" s="21">
         <v>123</v>
       </c>
-      <c r="B49" t="s" s="19">
+      <c r="B49" t="s" s="22">
         <v>124</v>
       </c>
-      <c r="C49" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s" s="19">
+      <c r="C49" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" t="s" s="19">
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H49" s="20"/>
+      <c r="H49" s="23"/>
       <c r="I49" s="10"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -3336,24 +3355,24 @@
       <c r="N49" s="3"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
-      <c r="A50" t="s" s="18">
+      <c r="A50" t="s" s="21">
         <v>125</v>
       </c>
-      <c r="B50" t="s" s="19">
+      <c r="B50" t="s" s="22">
         <v>126</v>
       </c>
-      <c r="C50" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D50" t="s" s="19">
+      <c r="C50" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" t="s" s="19">
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H50" s="20"/>
+      <c r="H50" s="23"/>
       <c r="I50" s="10"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -3362,24 +3381,24 @@
       <c r="N50" s="3"/>
     </row>
     <row r="51" ht="15.35" customHeight="1">
-      <c r="A51" t="s" s="18">
+      <c r="A51" t="s" s="21">
         <v>127</v>
       </c>
-      <c r="B51" t="s" s="19">
+      <c r="B51" t="s" s="22">
         <v>128</v>
       </c>
-      <c r="C51" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s" s="19">
+      <c r="C51" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" t="s" s="19">
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H51" s="20"/>
+      <c r="H51" s="23"/>
       <c r="I51" s="10"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -3388,24 +3407,24 @@
       <c r="N51" s="3"/>
     </row>
     <row r="52" ht="15.35" customHeight="1">
-      <c r="A52" t="s" s="18">
+      <c r="A52" t="s" s="21">
         <v>129</v>
       </c>
-      <c r="B52" t="s" s="19">
+      <c r="B52" t="s" s="22">
         <v>130</v>
       </c>
-      <c r="C52" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s" s="19">
+      <c r="C52" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" t="s" s="19">
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H52" s="20"/>
+      <c r="H52" s="23"/>
       <c r="I52" s="10"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -3414,25 +3433,25 @@
       <c r="N52" s="3"/>
     </row>
     <row r="53" ht="15.35" customHeight="1">
-      <c r="A53" t="s" s="18">
+      <c r="A53" t="s" s="21">
         <v>131</v>
       </c>
-      <c r="B53" t="s" s="19">
+      <c r="B53" t="s" s="22">
         <v>132</v>
       </c>
-      <c r="C53" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="D53" t="s" s="19">
+      <c r="C53" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s" s="22">
         <v>113</v>
       </c>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" t="s" s="19">
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" t="s" s="22">
         <v>114</v>
       </c>
-      <c r="H53" s="20"/>
-      <c r="I53" s="21"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="24"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
@@ -3440,132 +3459,132 @@
       <c r="N53" s="5"/>
     </row>
     <row r="54" ht="15.35" customHeight="1">
-      <c r="A54" t="s" s="22">
+      <c r="A54" t="s" s="25">
         <v>133</v>
       </c>
-      <c r="B54" t="s" s="23">
+      <c r="B54" t="s" s="26">
         <v>134</v>
       </c>
-      <c r="C54" t="s" s="23">
-        <v>9</v>
-      </c>
-      <c r="D54" t="s" s="23">
+      <c r="C54" t="s" s="26">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s" s="26">
         <v>135</v>
       </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" t="s" s="23">
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" t="s" s="26">
         <v>136</v>
       </c>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="25"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="28"/>
     </row>
     <row r="55" ht="15.35" customHeight="1">
-      <c r="A55" t="s" s="22">
+      <c r="A55" t="s" s="25">
         <v>137</v>
       </c>
-      <c r="B55" t="s" s="23">
+      <c r="B55" t="s" s="26">
         <v>138</v>
       </c>
-      <c r="C55" t="s" s="23">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s" s="23">
+      <c r="C55" t="s" s="26">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s" s="26">
         <v>135</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" t="s" s="23">
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" t="s" s="26">
         <v>136</v>
       </c>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="24"/>
-      <c r="N55" s="25"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="27"/>
+      <c r="N55" s="28"/>
     </row>
     <row r="56" ht="15.35" customHeight="1">
-      <c r="A56" t="s" s="22">
+      <c r="A56" t="s" s="29">
         <v>139</v>
       </c>
-      <c r="B56" t="s" s="23">
+      <c r="B56" t="s" s="26">
         <v>140</v>
       </c>
-      <c r="C56" t="s" s="23">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s" s="23">
+      <c r="C56" t="s" s="26">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s" s="26">
         <v>135</v>
       </c>
-      <c r="E56" t="s" s="23">
+      <c r="E56" t="s" s="26">
         <v>141</v>
       </c>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
-      <c r="J56" s="24"/>
-      <c r="K56" s="24"/>
-      <c r="L56" s="24"/>
-      <c r="M56" s="24"/>
-      <c r="N56" s="25"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="27"/>
+      <c r="N56" s="28"/>
     </row>
     <row r="57" ht="15.35" customHeight="1">
-      <c r="A57" t="s" s="26">
+      <c r="A57" t="s" s="30">
         <v>142</v>
       </c>
-      <c r="B57" t="s" s="27">
+      <c r="B57" t="s" s="31">
         <v>143</v>
       </c>
-      <c r="C57" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s" s="27">
+      <c r="C57" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E57" t="s" s="27">
+      <c r="E57" t="s" s="31">
         <v>145</v>
       </c>
-      <c r="F57" s="28"/>
-      <c r="G57" t="s" s="27">
+      <c r="F57" s="32"/>
+      <c r="G57" t="s" s="31">
         <v>146</v>
       </c>
-      <c r="H57" s="28"/>
-      <c r="I57" s="29"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="30"/>
-      <c r="M57" s="30"/>
-      <c r="N57" s="30"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
+      <c r="N57" s="34"/>
     </row>
     <row r="58" ht="15.35" customHeight="1">
-      <c r="A58" t="s" s="26">
+      <c r="A58" t="s" s="30">
         <v>147</v>
       </c>
-      <c r="B58" t="s" s="27">
+      <c r="B58" t="s" s="31">
         <v>148</v>
       </c>
-      <c r="C58" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D58" t="s" s="27">
+      <c r="C58" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E58" t="s" s="27">
+      <c r="E58" t="s" s="31">
         <v>149</v>
       </c>
-      <c r="F58" s="28"/>
-      <c r="G58" t="s" s="27">
+      <c r="F58" s="32"/>
+      <c r="G58" t="s" s="31">
         <v>150</v>
       </c>
-      <c r="H58" s="28"/>
+      <c r="H58" s="32"/>
       <c r="I58" s="10"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -3574,24 +3593,24 @@
       <c r="N58" s="3"/>
     </row>
     <row r="59" ht="15.35" customHeight="1">
-      <c r="A59" t="s" s="26">
+      <c r="A59" t="s" s="30">
         <v>151</v>
       </c>
-      <c r="B59" t="s" s="27">
+      <c r="B59" t="s" s="31">
         <v>152</v>
       </c>
-      <c r="C59" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D59" t="s" s="27">
+      <c r="C59" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E59" t="s" s="27">
+      <c r="E59" t="s" s="31">
         <v>149</v>
       </c>
-      <c r="F59" s="28"/>
-      <c r="G59" s="28"/>
-      <c r="H59" s="28"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
       <c r="I59" s="10"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -3600,24 +3619,24 @@
       <c r="N59" s="3"/>
     </row>
     <row r="60" ht="15.35" customHeight="1">
-      <c r="A60" t="s" s="26">
+      <c r="A60" t="s" s="30">
         <v>153</v>
       </c>
-      <c r="B60" t="s" s="27">
+      <c r="B60" t="s" s="31">
         <v>154</v>
       </c>
-      <c r="C60" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D60" t="s" s="27">
+      <c r="C60" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E60" t="s" s="27">
+      <c r="E60" t="s" s="31">
         <v>155</v>
       </c>
-      <c r="F60" s="28"/>
-      <c r="G60" s="28"/>
-      <c r="H60" s="28"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
       <c r="I60" s="10"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -3626,24 +3645,24 @@
       <c r="N60" s="3"/>
     </row>
     <row r="61" ht="15.35" customHeight="1">
-      <c r="A61" t="s" s="26">
+      <c r="A61" t="s" s="30">
         <v>156</v>
       </c>
-      <c r="B61" t="s" s="27">
+      <c r="B61" t="s" s="31">
         <v>157</v>
       </c>
-      <c r="C61" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D61" t="s" s="27">
+      <c r="C61" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E61" t="s" s="27">
+      <c r="E61" t="s" s="31">
         <v>155</v>
       </c>
-      <c r="F61" s="28"/>
-      <c r="G61" s="28"/>
-      <c r="H61" s="28"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="32"/>
       <c r="I61" s="10"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
@@ -3652,24 +3671,24 @@
       <c r="N61" s="3"/>
     </row>
     <row r="62" ht="15.35" customHeight="1">
-      <c r="A62" t="s" s="31">
+      <c r="A62" t="s" s="35">
         <v>158</v>
       </c>
-      <c r="B62" t="s" s="27">
+      <c r="B62" t="s" s="31">
         <v>159</v>
       </c>
-      <c r="C62" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D62" t="s" s="27">
+      <c r="C62" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E62" t="s" s="27">
+      <c r="E62" t="s" s="31">
         <v>155</v>
       </c>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
       <c r="I62" s="10"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
@@ -3678,24 +3697,24 @@
       <c r="N62" s="3"/>
     </row>
     <row r="63" ht="15.35" customHeight="1">
-      <c r="A63" t="s" s="26">
+      <c r="A63" t="s" s="30">
         <v>160</v>
       </c>
-      <c r="B63" t="s" s="27">
+      <c r="B63" t="s" s="31">
         <v>161</v>
       </c>
-      <c r="C63" t="s" s="27">
-        <v>9</v>
-      </c>
-      <c r="D63" t="s" s="27">
+      <c r="C63" t="s" s="31">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s" s="31">
         <v>144</v>
       </c>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
-      <c r="G63" t="s" s="27">
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" t="s" s="31">
         <v>162</v>
       </c>
-      <c r="H63" s="28"/>
+      <c r="H63" s="32"/>
       <c r="I63" s="10"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -3704,28 +3723,28 @@
       <c r="N63" s="3"/>
     </row>
     <row r="64" ht="15.35" customHeight="1">
-      <c r="A64" t="s" s="32">
+      <c r="A64" t="s" s="36">
         <v>163</v>
       </c>
-      <c r="B64" t="s" s="33">
+      <c r="B64" t="s" s="37">
         <v>164</v>
       </c>
-      <c r="C64" t="s" s="33">
-        <v>9</v>
-      </c>
-      <c r="D64" t="s" s="33">
+      <c r="C64" t="s" s="37">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s" s="37">
         <v>165</v>
       </c>
-      <c r="E64" t="s" s="33">
+      <c r="E64" t="s" s="37">
         <v>166</v>
       </c>
-      <c r="F64" t="s" s="33">
+      <c r="F64" t="s" s="37">
         <v>167</v>
       </c>
-      <c r="G64" t="s" s="33">
+      <c r="G64" t="s" s="37">
         <v>168</v>
       </c>
-      <c r="H64" s="34"/>
+      <c r="H64" s="38"/>
       <c r="I64" s="10"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
@@ -3734,28 +3753,28 @@
       <c r="N64" s="3"/>
     </row>
     <row r="65" ht="15.35" customHeight="1">
-      <c r="A65" t="s" s="32">
+      <c r="A65" t="s" s="36">
         <v>169</v>
       </c>
-      <c r="B65" t="s" s="33">
+      <c r="B65" t="s" s="37">
         <v>170</v>
       </c>
-      <c r="C65" t="s" s="33">
-        <v>9</v>
-      </c>
-      <c r="D65" t="s" s="33">
+      <c r="C65" t="s" s="37">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s" s="37">
         <v>165</v>
       </c>
-      <c r="E65" t="s" s="33">
+      <c r="E65" t="s" s="37">
         <v>16</v>
       </c>
-      <c r="F65" t="s" s="33">
+      <c r="F65" t="s" s="37">
         <v>167</v>
       </c>
-      <c r="G65" t="s" s="33">
+      <c r="G65" t="s" s="37">
         <v>168</v>
       </c>
-      <c r="H65" s="34"/>
+      <c r="H65" s="38"/>
       <c r="I65" s="10"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
@@ -3764,14 +3783,14 @@
       <c r="N65" s="3"/>
     </row>
     <row r="66" ht="15.35" customHeight="1">
-      <c r="A66" s="35"/>
-      <c r="B66" s="36"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="36"/>
+      <c r="A66" s="39"/>
+      <c r="B66" s="40"/>
+      <c r="C66" s="41"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="40"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="40"/>
       <c r="I66" s="10"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>

</xml_diff>